<commit_message>
hr dump import update
</commit_message>
<xml_diff>
--- a/public/sample/Spine HR dump.xlsx
+++ b/public/sample/Spine HR dump.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Frontier Projects\courier.register\public\sample\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\FR-CHD-00110\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{509EDF10-2B8E-4955-8809-4C610B04271B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{38DCD07A-F3F6-4746-8D95-843B9137BC20}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="138">
   <si>
     <t/>
   </si>
@@ -136,9 +136,6 @@
     <t>00034</t>
   </si>
   <si>
-    <t>FAPL_Unit_3</t>
-  </si>
-  <si>
     <t>FAGSD-00266</t>
   </si>
   <si>
@@ -404,6 +401,39 @@
   </si>
   <si>
     <t>FEROZEPUR</t>
+  </si>
+  <si>
+    <t>10026</t>
+  </si>
+  <si>
+    <t>MA2</t>
+  </si>
+  <si>
+    <t>10048</t>
+  </si>
+  <si>
+    <t>SD1</t>
+  </si>
+  <si>
+    <t>10059</t>
+  </si>
+  <si>
+    <t>IAG Code</t>
+  </si>
+  <si>
+    <t>PFU</t>
+  </si>
+  <si>
+    <t>10065</t>
+  </si>
+  <si>
+    <t>10086</t>
+  </si>
+  <si>
+    <t>FAPL_Unit_2</t>
+  </si>
+  <si>
+    <t>FAPL_Unit_1</t>
   </si>
 </sst>
 </file>
@@ -442,8 +472,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -758,47 +788,50 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AJ6"/>
+  <dimension ref="A1:AL6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13:B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.90625" customWidth="1"/>
-    <col min="2" max="3" width="15.6328125" customWidth="1"/>
-    <col min="4" max="4" width="37.7265625" customWidth="1"/>
-    <col min="5" max="5" width="44.1796875" customWidth="1"/>
-    <col min="6" max="7" width="23.36328125" customWidth="1"/>
-    <col min="8" max="8" width="18.1796875" customWidth="1"/>
-    <col min="9" max="9" width="32.453125" customWidth="1"/>
-    <col min="10" max="11" width="19.453125" customWidth="1"/>
-    <col min="12" max="12" width="10.36328125" customWidth="1"/>
-    <col min="13" max="13" width="16.90625" customWidth="1"/>
-    <col min="14" max="14" width="29.90625" customWidth="1"/>
-    <col min="15" max="15" width="9.08984375" customWidth="1"/>
-    <col min="16" max="16" width="18.1796875" customWidth="1"/>
-    <col min="17" max="17" width="14.26953125" customWidth="1"/>
-    <col min="18" max="19" width="52" customWidth="1"/>
-    <col min="20" max="20" width="16.90625" customWidth="1"/>
-    <col min="21" max="22" width="14.26953125" customWidth="1"/>
-    <col min="23" max="23" width="27.26953125" customWidth="1"/>
-    <col min="24" max="24" width="13" customWidth="1"/>
-    <col min="25" max="25" width="14.26953125" customWidth="1"/>
-    <col min="26" max="26" width="16.90625" customWidth="1"/>
-    <col min="27" max="27" width="22.08984375" customWidth="1"/>
-    <col min="28" max="28" width="16.90625" customWidth="1"/>
-    <col min="29" max="29" width="50.7265625" customWidth="1"/>
-    <col min="30" max="30" width="37.7265625" customWidth="1"/>
-    <col min="31" max="31" width="13" customWidth="1"/>
-    <col min="32" max="33" width="11.7265625" customWidth="1"/>
-    <col min="34" max="34" width="20.81640625" customWidth="1"/>
-    <col min="35" max="35" width="16.90625" customWidth="1"/>
-    <col min="36" max="36" width="20.81640625" customWidth="1"/>
+    <col min="1" max="1" width="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="11" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="37" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="7.7109375" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="33" max="35" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="15" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:38">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -812,639 +845,669 @@
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AG1" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AH1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="AJ1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:38">
       <c r="A2" t="s">
         <v>37</v>
       </c>
       <c r="B2" t="s">
+        <v>136</v>
+      </c>
+      <c r="C2" t="s">
         <v>38</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>39</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>128</v>
+      </c>
+      <c r="G2" t="s">
         <v>40</v>
       </c>
-      <c r="E2" t="s">
+      <c r="H2" t="s">
         <v>41</v>
       </c>
-      <c r="F2" t="s">
+      <c r="I2" t="s">
         <v>42</v>
       </c>
-      <c r="G2" t="s">
+      <c r="J2" t="s">
+        <v>42</v>
+      </c>
+      <c r="K2" t="s">
         <v>43</v>
       </c>
-      <c r="H2" t="s">
+      <c r="L2" t="s">
+        <v>44</v>
+      </c>
+      <c r="M2" t="s">
+        <v>45</v>
+      </c>
+      <c r="N2" t="s">
+        <v>46</v>
+      </c>
+      <c r="O2" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>49</v>
+      </c>
+      <c r="R2" t="s">
+        <v>50</v>
+      </c>
+      <c r="S2" t="s">
+        <v>51</v>
+      </c>
+      <c r="T2" t="s">
+        <v>52</v>
+      </c>
+      <c r="U2" t="s">
+        <v>53</v>
+      </c>
+      <c r="V2" t="s">
+        <v>54</v>
+      </c>
+      <c r="W2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X2" t="s">
+        <v>56</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>57</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>59</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>60</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38">
+      <c r="A3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B3" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G3" t="s">
+        <v>68</v>
+      </c>
+      <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K3" t="s">
         <v>43</v>
       </c>
-      <c r="I2" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" t="s">
-        <v>45</v>
-      </c>
-      <c r="K2" t="s">
+      <c r="L3" t="s">
+        <v>71</v>
+      </c>
+      <c r="M3" t="s">
+        <v>72</v>
+      </c>
+      <c r="N3" t="s">
         <v>46</v>
       </c>
-      <c r="L2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="O3" t="s">
+        <v>73</v>
+      </c>
+      <c r="P3" t="s">
         <v>48</v>
       </c>
-      <c r="N2" t="s">
+      <c r="Q3" t="s">
         <v>49</v>
       </c>
-      <c r="O2" t="s">
+      <c r="R3" t="s">
         <v>50</v>
       </c>
-      <c r="P2" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>52</v>
-      </c>
-      <c r="R2" t="s">
-        <v>53</v>
-      </c>
-      <c r="S2" t="s">
-        <v>54</v>
-      </c>
-      <c r="T2" t="s">
-        <v>55</v>
-      </c>
-      <c r="U2" t="s">
-        <v>56</v>
-      </c>
-      <c r="V2" t="s">
+      <c r="S3" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" t="s">
+        <v>76</v>
+      </c>
+      <c r="V3" t="s">
+        <v>77</v>
+      </c>
+      <c r="W3" t="s">
+        <v>78</v>
+      </c>
+      <c r="X3" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>80</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>81</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>82</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>83</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF3" t="s">
+        <v>84</v>
+      </c>
+      <c r="AG3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK3" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38">
+      <c r="A4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B4" t="s">
+        <v>136</v>
+      </c>
+      <c r="C4" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" t="s">
+        <v>87</v>
+      </c>
+      <c r="E4" t="s">
+        <v>131</v>
+      </c>
+      <c r="F4" t="s">
+        <v>128</v>
+      </c>
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
+        <v>88</v>
+      </c>
+      <c r="I4" t="s">
+        <v>70</v>
+      </c>
+      <c r="J4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K4" t="s">
+        <v>43</v>
+      </c>
+      <c r="L4" t="s">
+        <v>71</v>
+      </c>
+      <c r="M4" t="s">
+        <v>0</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
+      </c>
+      <c r="O4" t="s">
+        <v>89</v>
+      </c>
+      <c r="P4" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>49</v>
+      </c>
+      <c r="R4" t="s">
+        <v>50</v>
+      </c>
+      <c r="S4" t="s">
+        <v>90</v>
+      </c>
+      <c r="T4" t="s">
+        <v>91</v>
+      </c>
+      <c r="U4" t="s">
+        <v>92</v>
+      </c>
+      <c r="V4" t="s">
+        <v>93</v>
+      </c>
+      <c r="W4" t="s">
+        <v>78</v>
+      </c>
+      <c r="X4" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>79</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>94</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC4" t="s">
+        <v>96</v>
+      </c>
+      <c r="AD4" t="s">
+        <v>62</v>
+      </c>
+      <c r="AE4" t="s">
+        <v>63</v>
+      </c>
+      <c r="AF4" t="s">
+        <v>64</v>
+      </c>
+      <c r="AG4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK4" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38">
+      <c r="A5" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C5" t="s">
+        <v>98</v>
+      </c>
+      <c r="D5" t="s">
+        <v>99</v>
+      </c>
+      <c r="E5" t="s">
+        <v>134</v>
+      </c>
+      <c r="F5" t="s">
+        <v>128</v>
+      </c>
+      <c r="G5" t="s">
+        <v>68</v>
+      </c>
+      <c r="H5" t="s">
+        <v>100</v>
+      </c>
+      <c r="I5" t="s">
+        <v>42</v>
+      </c>
+      <c r="J5" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" t="s">
+        <v>43</v>
+      </c>
+      <c r="L5" t="s">
+        <v>71</v>
+      </c>
+      <c r="M5" t="s">
+        <v>0</v>
+      </c>
+      <c r="N5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O5" t="s">
+        <v>101</v>
+      </c>
+      <c r="P5" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>49</v>
+      </c>
+      <c r="R5" t="s">
+        <v>50</v>
+      </c>
+      <c r="S5" t="s">
+        <v>102</v>
+      </c>
+      <c r="T5" t="s">
+        <v>103</v>
+      </c>
+      <c r="U5" t="s">
+        <v>104</v>
+      </c>
+      <c r="V5" t="s">
+        <v>105</v>
+      </c>
+      <c r="W5" t="s">
+        <v>78</v>
+      </c>
+      <c r="X5" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y5" t="s">
         <v>57</v>
       </c>
-      <c r="W2" t="s">
+      <c r="Z5" t="s">
         <v>58</v>
       </c>
-      <c r="X2" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>60</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>61</v>
-      </c>
-      <c r="AA2" t="s">
+      <c r="AA5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AB5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AC5" t="s">
+        <v>108</v>
+      </c>
+      <c r="AD5" t="s">
         <v>62</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AE5" t="s">
         <v>63</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AF5" t="s">
         <v>64</v>
       </c>
-      <c r="AD2" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ2" t="s">
+      <c r="AG5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AH5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AI5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AJ5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
-      <c r="A3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" t="s">
-        <v>38</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" t="s">
-        <v>68</v>
-      </c>
-      <c r="E3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F3" t="s">
-        <v>70</v>
-      </c>
-      <c r="G3" t="s">
+    <row r="6" spans="1:38">
+      <c r="A6" t="s">
+        <v>109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>136</v>
+      </c>
+      <c r="C6" t="s">
+        <v>110</v>
+      </c>
+      <c r="D6" t="s">
+        <v>111</v>
+      </c>
+      <c r="E6" t="s">
+        <v>135</v>
+      </c>
+      <c r="F6" t="s">
+        <v>128</v>
+      </c>
+      <c r="G6" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" t="s">
+        <v>113</v>
+      </c>
+      <c r="I6" t="s">
+        <v>114</v>
+      </c>
+      <c r="J6" t="s">
+        <v>114</v>
+      </c>
+      <c r="K6" t="s">
+        <v>43</v>
+      </c>
+      <c r="L6" t="s">
         <v>71</v>
       </c>
-      <c r="H3" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" t="s">
-        <v>72</v>
-      </c>
-      <c r="K3" t="s">
-        <v>73</v>
-      </c>
-      <c r="L3" t="s">
-        <v>47</v>
-      </c>
-      <c r="M3" t="s">
-        <v>74</v>
-      </c>
-      <c r="N3" t="s">
+      <c r="M6" t="s">
+        <v>0</v>
+      </c>
+      <c r="N6" t="s">
+        <v>46</v>
+      </c>
+      <c r="O6" t="s">
+        <v>115</v>
+      </c>
+      <c r="P6" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q6" t="s">
         <v>49</v>
       </c>
-      <c r="O3" t="s">
+      <c r="R6" t="s">
         <v>50</v>
       </c>
-      <c r="P3" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>75</v>
-      </c>
-      <c r="R3" t="s">
-        <v>76</v>
-      </c>
-      <c r="S3" t="s">
-        <v>77</v>
-      </c>
-      <c r="T3" t="s">
+      <c r="S6" t="s">
+        <v>116</v>
+      </c>
+      <c r="T6" t="s">
+        <v>117</v>
+      </c>
+      <c r="U6" t="s">
+        <v>118</v>
+      </c>
+      <c r="V6" t="s">
+        <v>119</v>
+      </c>
+      <c r="W6" t="s">
         <v>78</v>
       </c>
-      <c r="U3" t="s">
-        <v>79</v>
-      </c>
-      <c r="V3" t="s">
-        <v>0</v>
-      </c>
-      <c r="W3" t="s">
-        <v>80</v>
-      </c>
-      <c r="X3" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>81</v>
-      </c>
-      <c r="Z3" t="s">
-        <v>82</v>
-      </c>
-      <c r="AA3" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB3" t="s">
-        <v>84</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>85</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI3" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:36">
-      <c r="A4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B4" t="s">
-        <v>38</v>
-      </c>
-      <c r="C4" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F4" t="s">
-        <v>89</v>
-      </c>
-      <c r="G4" t="s">
-        <v>71</v>
-      </c>
-      <c r="H4" t="s">
-        <v>71</v>
-      </c>
-      <c r="I4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J4" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" t="s">
-        <v>0</v>
-      </c>
-      <c r="L4" t="s">
-        <v>47</v>
-      </c>
-      <c r="M4" t="s">
-        <v>90</v>
-      </c>
-      <c r="N4" t="s">
-        <v>49</v>
-      </c>
-      <c r="O4" t="s">
-        <v>50</v>
-      </c>
-      <c r="P4" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>91</v>
-      </c>
-      <c r="R4" t="s">
-        <v>92</v>
-      </c>
-      <c r="S4" t="s">
-        <v>93</v>
-      </c>
-      <c r="T4" t="s">
-        <v>94</v>
-      </c>
-      <c r="U4" t="s">
-        <v>79</v>
-      </c>
-      <c r="V4" t="s">
-        <v>0</v>
-      </c>
-      <c r="W4" t="s">
-        <v>80</v>
-      </c>
-      <c r="X4" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y4" t="s">
-        <v>95</v>
-      </c>
-      <c r="Z4" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA4" t="s">
-        <v>97</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC4" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD4" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI4" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ4" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:36">
-      <c r="A5" t="s">
-        <v>98</v>
-      </c>
-      <c r="B5" t="s">
-        <v>38</v>
-      </c>
-      <c r="C5" t="s">
-        <v>99</v>
-      </c>
-      <c r="D5" t="s">
-        <v>100</v>
-      </c>
-      <c r="E5" t="s">
-        <v>69</v>
-      </c>
-      <c r="F5" t="s">
-        <v>101</v>
-      </c>
-      <c r="G5" t="s">
-        <v>43</v>
-      </c>
-      <c r="H5" t="s">
-        <v>43</v>
-      </c>
-      <c r="I5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K5" t="s">
-        <v>0</v>
-      </c>
-      <c r="L5" t="s">
-        <v>47</v>
-      </c>
-      <c r="M5" t="s">
-        <v>102</v>
-      </c>
-      <c r="N5" t="s">
-        <v>49</v>
-      </c>
-      <c r="O5" t="s">
-        <v>50</v>
-      </c>
-      <c r="P5" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>103</v>
-      </c>
-      <c r="R5" t="s">
-        <v>104</v>
-      </c>
-      <c r="S5" t="s">
-        <v>105</v>
-      </c>
-      <c r="T5" t="s">
-        <v>106</v>
-      </c>
-      <c r="U5" t="s">
-        <v>79</v>
-      </c>
-      <c r="V5" t="s">
-        <v>0</v>
-      </c>
-      <c r="W5" t="s">
+      <c r="X6" t="s">
+        <v>0</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z6" t="s">
         <v>58</v>
       </c>
-      <c r="X5" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y5" t="s">
-        <v>107</v>
-      </c>
-      <c r="Z5" t="s">
-        <v>108</v>
-      </c>
-      <c r="AA5" t="s">
-        <v>109</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>63</v>
-      </c>
-      <c r="AC5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AD5" t="s">
-        <v>65</v>
-      </c>
-      <c r="AE5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AG5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AH5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AI5" t="s">
-        <v>0</v>
-      </c>
-      <c r="AJ5" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:36">
-      <c r="A6" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C6" t="s">
-        <v>111</v>
-      </c>
-      <c r="D6" t="s">
-        <v>112</v>
-      </c>
-      <c r="E6" t="s">
-        <v>113</v>
-      </c>
-      <c r="F6" t="s">
-        <v>114</v>
-      </c>
-      <c r="G6" t="s">
-        <v>115</v>
-      </c>
-      <c r="H6" t="s">
-        <v>115</v>
-      </c>
-      <c r="I6" t="s">
-        <v>44</v>
-      </c>
-      <c r="J6" t="s">
-        <v>72</v>
-      </c>
-      <c r="K6" t="s">
-        <v>0</v>
-      </c>
-      <c r="L6" t="s">
-        <v>47</v>
-      </c>
-      <c r="M6" t="s">
-        <v>116</v>
-      </c>
-      <c r="N6" t="s">
-        <v>49</v>
-      </c>
-      <c r="O6" t="s">
-        <v>50</v>
-      </c>
-      <c r="P6" t="s">
-        <v>51</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>117</v>
-      </c>
-      <c r="R6" t="s">
-        <v>118</v>
-      </c>
-      <c r="S6" t="s">
-        <v>119</v>
-      </c>
-      <c r="T6" t="s">
-        <v>120</v>
-      </c>
-      <c r="U6" t="s">
-        <v>79</v>
-      </c>
-      <c r="V6" t="s">
-        <v>0</v>
-      </c>
-      <c r="W6" t="s">
+      <c r="AA6" t="s">
         <v>121</v>
       </c>
-      <c r="X6" t="s">
-        <v>59</v>
-      </c>
-      <c r="Y6" t="s">
+      <c r="AB6" t="s">
         <v>122</v>
       </c>
-      <c r="Z6" t="s">
+      <c r="AC6" t="s">
         <v>123</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AD6" t="s">
         <v>124</v>
       </c>
-      <c r="AB6" t="s">
+      <c r="AE6" t="s">
         <v>125</v>
       </c>
-      <c r="AC6" t="s">
+      <c r="AF6" t="s">
         <v>126</v>
       </c>
-      <c r="AD6" t="s">
-        <v>127</v>
-      </c>
-      <c r="AE6" t="s">
-        <v>0</v>
-      </c>
-      <c r="AF6" t="s">
-        <v>0</v>
-      </c>
       <c r="AG6" t="s">
         <v>0</v>
       </c>
@@ -1455,6 +1518,12 @@
         <v>0</v>
       </c>
       <c r="AJ6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>0</v>
+      </c>
+      <c r="AL6" t="s">
         <v>0</v>
       </c>
     </row>

</xml_diff>